<commit_message>
Changes for the demo version
</commit_message>
<xml_diff>
--- a/ContactTracing15/ContactTracingReport.xlsx
+++ b/ContactTracing15/ContactTracingReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -99,6 +99,12 @@
     <x:t>04/05/2021 00:00:00</x:t>
   </x:si>
   <x:si>
+    <x:t>OX2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 23:42:46</x:t>
+  </x:si>
+  <x:si>
     <x:t>CaseId</x:t>
   </x:si>
   <x:si>
@@ -109,6 +115,9 @@
   </x:si>
   <x:si>
     <x:t>04/05/2021 21:45:31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 23:42:13</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -242,8 +251,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cases" displayName="Cases" ref="A1:J5" totalsRowShown="0">
-  <x:autoFilter ref="A1:J5"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cases" displayName="Cases" ref="A1:J6" totalsRowShown="0">
+  <x:autoFilter ref="A1:J6"/>
   <x:tableColumns count="10">
     <x:tableColumn id="1" name="Id"/>
     <x:tableColumn id="2" name="Test Date" dataDxfId="0"/>
@@ -261,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Contacts" displayName="Contacts" ref="A1:F3" totalsRowShown="0">
-  <x:autoFilter ref="A1:F3"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Contacts" displayName="Contacts" ref="A1:F4" totalsRowShown="0">
+  <x:autoFilter ref="A1:F4"/>
   <x:tableColumns count="6">
     <x:tableColumn id="1" name="Id"/>
     <x:tableColumn id="2" name="CaseId"/>
@@ -783,7 +792,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J5"/>
+  <x:dimension ref="A1:J6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -920,6 +929,32 @@
       </x:c>
       <x:c r="I5" s="0" t="s">
         <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10">
+      <x:c r="A6" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C6" s="2">
+        <x:v>44320.987027581</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -938,7 +973,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F3"/>
+  <x:dimension ref="A1:F4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -949,7 +984,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
         <x:v>15</x:v>
@@ -958,7 +993,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
         <x:v>21</x:v>
@@ -978,7 +1013,7 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
@@ -995,7 +1030,24 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="2">
+        <x:v>44320.9875444792</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
tried making the table scrollable, nothing changed
</commit_message>
<xml_diff>
--- a/ContactTracing15/ContactTracingReport.xlsx
+++ b/ContactTracing15/ContactTracingReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -87,28 +87,19 @@
     <x:t>Removed date</x:t>
   </x:si>
   <x:si>
-    <x:t>CB5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>04/05/2021 08:54:13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>04/05/2021 21:46:23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>04/05/2021 00:00:00</x:t>
+    <x:t>4/30/2021 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/1/2021 12:00:00 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5/11/2021 12:00:00 AM</x:t>
   </x:si>
   <x:si>
     <x:t>CaseId</x:t>
   </x:si>
   <x:si>
     <x:t>Contacted date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>04/05/2021 08:54:06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>04/05/2021 21:45:31</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -242,8 +233,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cases" displayName="Cases" ref="A1:J5" totalsRowShown="0">
-  <x:autoFilter ref="A1:J5"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cases" displayName="Cases" ref="A1:J23" totalsRowShown="0">
+  <x:autoFilter ref="A1:J23"/>
   <x:tableColumns count="10">
     <x:tableColumn id="1" name="Id"/>
     <x:tableColumn id="2" name="Test Date" dataDxfId="0"/>
@@ -783,7 +774,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J5"/>
+  <x:dimension ref="A1:J23"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -826,25 +817,25 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="1">
-        <x:v>44320</x:v>
+        <x:v>44317</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>44320.3700041551</x:v>
+        <x:v>44317.9528023727</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
         <x:v>22</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="b">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -852,10 +843,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="1">
-        <x:v>44320</x:v>
+        <x:v>44317</x:v>
       </x:c>
       <x:c r="C3" s="2">
-        <x:v>44320.370304294</x:v>
+        <x:v>44317.9534171065</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>4</x:v>
@@ -868,6 +859,9 @@
       </x:c>
       <x:c r="G3" s="0" t="b">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -875,39 +869,36 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1">
-        <x:v>44321</x:v>
+        <x:v>44317</x:v>
       </x:c>
       <x:c r="C4" s="2">
-        <x:v>44320.9039171296</x:v>
+        <x:v>44317.9625158681</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="E4" s="0" t="b">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G4" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:10">
       <x:c r="A5" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>1002</x:v>
       </x:c>
       <x:c r="B5" s="1">
-        <x:v>44321</x:v>
+        <x:v>44327</x:v>
       </x:c>
       <x:c r="C5" s="2">
-        <x:v>44320.904597662</x:v>
+        <x:v>44327.7865993403</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E5" s="0" t="b">
         <x:v>0</x:v>
@@ -919,7 +910,448 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10">
+      <x:c r="A6" s="0" t="n">
+        <x:v>1003</x:v>
+      </x:c>
+      <x:c r="B6" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C6" s="2">
+        <x:v>44327.7869098611</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="A7" s="0" t="n">
+        <x:v>1004</x:v>
+      </x:c>
+      <x:c r="B7" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C7" s="2">
+        <x:v>44327.7871325463</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:10">
+      <x:c r="A8" s="0" t="n">
+        <x:v>1005</x:v>
+      </x:c>
+      <x:c r="B8" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C8" s="2">
+        <x:v>44327.7874183102</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
+      <x:c r="A9" s="0" t="n">
+        <x:v>1006</x:v>
+      </x:c>
+      <x:c r="B9" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C9" s="2">
+        <x:v>44327.7876739699</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="A10" s="0" t="n">
+        <x:v>1007</x:v>
+      </x:c>
+      <x:c r="B10" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C10" s="2">
+        <x:v>44327.7878651042</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:10">
+      <x:c r="A11" s="0" t="n">
+        <x:v>1008</x:v>
+      </x:c>
+      <x:c r="B11" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C11" s="2">
+        <x:v>44327.7881653935</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:10">
+      <x:c r="A12" s="0" t="n">
+        <x:v>1009</x:v>
+      </x:c>
+      <x:c r="B12" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C12" s="2">
+        <x:v>44327.7885158333</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:10">
+      <x:c r="A13" s="0" t="n">
+        <x:v>1010</x:v>
+      </x:c>
+      <x:c r="B13" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C13" s="2">
+        <x:v>44327.7887260648</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:10">
+      <x:c r="A14" s="0" t="n">
+        <x:v>1011</x:v>
+      </x:c>
+      <x:c r="B14" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C14" s="2">
+        <x:v>44327.7889103241</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:10">
+      <x:c r="A15" s="0" t="n">
+        <x:v>1012</x:v>
+      </x:c>
+      <x:c r="B15" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C15" s="2">
+        <x:v>44327.7896717014</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:10">
+      <x:c r="A16" s="0" t="n">
+        <x:v>1013</x:v>
+      </x:c>
+      <x:c r="B16" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C16" s="2">
+        <x:v>44327.7898875116</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:10">
+      <x:c r="A17" s="0" t="n">
+        <x:v>1014</x:v>
+      </x:c>
+      <x:c r="B17" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C17" s="2">
+        <x:v>44327.7900773148</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:10">
+      <x:c r="A18" s="0" t="n">
+        <x:v>1015</x:v>
+      </x:c>
+      <x:c r="B18" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C18" s="2">
+        <x:v>44327.7902346644</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:10">
+      <x:c r="A19" s="0" t="n">
+        <x:v>1016</x:v>
+      </x:c>
+      <x:c r="B19" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C19" s="2">
+        <x:v>44327.7905140393</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:10">
+      <x:c r="A20" s="0" t="n">
+        <x:v>1017</x:v>
+      </x:c>
+      <x:c r="B20" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C20" s="2">
+        <x:v>44327.7906821875</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:10">
+      <x:c r="A21" s="0" t="n">
+        <x:v>1018</x:v>
+      </x:c>
+      <x:c r="B21" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C21" s="2">
+        <x:v>44327.7908281944</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:10">
+      <x:c r="A22" s="0" t="n">
+        <x:v>1019</x:v>
+      </x:c>
+      <x:c r="B22" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C22" s="2">
+        <x:v>44327.7909767708</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:10">
+      <x:c r="A23" s="0" t="n">
+        <x:v>1020</x:v>
+      </x:c>
+      <x:c r="B23" s="1">
+        <x:v>44327</x:v>
+      </x:c>
+      <x:c r="C23" s="2">
+        <x:v>44327.7911247338</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G23" s="0" t="b">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -949,7 +1381,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
         <x:v>15</x:v>
@@ -958,7 +1390,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
         <x:v>21</x:v>
@@ -966,36 +1398,24 @@
     </x:row>
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>44320.3708740625</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>44319.7581985185</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
       <x:c r="C3" s="2">
-        <x:v>44320.9065409606</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>44319.7585063773</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Make table scrollable (2)
</commit_message>
<xml_diff>
--- a/ContactTracing15/ContactTracingReport.xlsx
+++ b/ContactTracing15/ContactTracingReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -87,19 +87,40 @@
     <x:t>Removed date</x:t>
   </x:si>
   <x:si>
-    <x:t>4/30/2021 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5/1/2021 12:00:00 AM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5/11/2021 12:00:00 AM</x:t>
+    <x:t>CB5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 08:54:13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11/05/2021 21:45:11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 21:46:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OX2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 23:42:46</x:t>
   </x:si>
   <x:si>
     <x:t>CaseId</x:t>
   </x:si>
   <x:si>
     <x:t>Contacted date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 08:54:06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 21:45:31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>04/05/2021 23:42:13</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -233,8 +254,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cases" displayName="Cases" ref="A1:J23" totalsRowShown="0">
-  <x:autoFilter ref="A1:J23"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cases" displayName="Cases" ref="A1:J36" totalsRowShown="0">
+  <x:autoFilter ref="A1:J36"/>
   <x:tableColumns count="10">
     <x:tableColumn id="1" name="Id"/>
     <x:tableColumn id="2" name="Test Date" dataDxfId="0"/>
@@ -252,8 +273,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Contacts" displayName="Contacts" ref="A1:F3" totalsRowShown="0">
-  <x:autoFilter ref="A1:F3"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Contacts" displayName="Contacts" ref="A1:F5" totalsRowShown="0">
+  <x:autoFilter ref="A1:F5"/>
   <x:tableColumns count="6">
     <x:tableColumn id="1" name="Id"/>
     <x:tableColumn id="2" name="CaseId"/>
@@ -774,7 +795,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J23"/>
+  <x:dimension ref="A1:J36"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -817,16 +838,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="1">
-        <x:v>44317</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>44317.9528023727</x:v>
+        <x:v>44320.3700041551</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E2" s="0" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F2" s="0" t="n">
         <x:v>0</x:v>
@@ -834,8 +855,8 @@
       <x:c r="G2" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
-        <x:v>22</x:v>
+      <x:c r="H2" s="0" t="s">
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -843,16 +864,16 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="1">
-        <x:v>44317</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C3" s="2">
-        <x:v>44317.9534171065</x:v>
+        <x:v>44320.370304294</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="E3" s="0" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F3" s="0" t="n">
         <x:v>0</x:v>
@@ -860,8 +881,8 @@
       <x:c r="G3" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>23</x:v>
+      <x:c r="H3" s="0" t="s">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -869,36 +890,39 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1">
-        <x:v>44317</x:v>
+        <x:v>44321</x:v>
       </x:c>
       <x:c r="C4" s="2">
-        <x:v>44317.9625158681</x:v>
+        <x:v>44320.9039171296</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="E4" s="0" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="G4" s="0" t="b">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:10">
       <x:c r="A5" s="0" t="n">
-        <x:v>1002</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="1">
-        <x:v>44327</x:v>
+        <x:v>44321</x:v>
       </x:c>
       <x:c r="C5" s="2">
-        <x:v>44327.7865993403</x:v>
+        <x:v>44320.904597662</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E5" s="0" t="b">
         <x:v>0</x:v>
@@ -910,24 +934,24 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="0" t="n">
-        <x:v>1003</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C6" s="2">
-        <x:v>44327.7869098611</x:v>
+        <x:v>44320.987027581</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E6" s="0" t="b">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="F6" s="0" t="n">
         <x:v>0</x:v>
@@ -935,22 +959,22 @@
       <x:c r="G6" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="I6" s="0" t="s">
-        <x:v>24</x:v>
+      <x:c r="H6" s="0" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10">
       <x:c r="A7" s="0" t="n">
-        <x:v>1004</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="1">
-        <x:v>44327</x:v>
+        <x:v>44321</x:v>
       </x:c>
       <x:c r="C7" s="2">
-        <x:v>44327.7871325463</x:v>
+        <x:v>44320.9045949074</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E7" s="0" t="b">
         <x:v>0</x:v>
@@ -962,18 +986,18 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10">
       <x:c r="A8" s="0" t="n">
-        <x:v>1005</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C8" s="2">
-        <x:v>44327.7874183102</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>4</x:v>
@@ -986,20 +1010,17 @@
       </x:c>
       <x:c r="G8" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I8" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10">
       <x:c r="A9" s="0" t="n">
-        <x:v>1006</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C9" s="2">
-        <x:v>44327.7876739699</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>4</x:v>
@@ -1012,20 +1033,17 @@
       </x:c>
       <x:c r="G9" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I9" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:10">
       <x:c r="A10" s="0" t="n">
-        <x:v>1007</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C10" s="2">
-        <x:v>44327.7878651042</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>4</x:v>
@@ -1038,20 +1056,17 @@
       </x:c>
       <x:c r="G10" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I10" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10">
       <x:c r="A11" s="0" t="n">
-        <x:v>1008</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C11" s="2">
-        <x:v>44327.7881653935</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>4</x:v>
@@ -1064,20 +1079,17 @@
       </x:c>
       <x:c r="G11" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I11" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10">
       <x:c r="A12" s="0" t="n">
-        <x:v>1009</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C12" s="2">
-        <x:v>44327.7885158333</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>4</x:v>
@@ -1090,20 +1102,17 @@
       </x:c>
       <x:c r="G12" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I12" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10">
       <x:c r="A13" s="0" t="n">
-        <x:v>1010</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C13" s="2">
-        <x:v>44327.7887260648</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>4</x:v>
@@ -1116,20 +1125,17 @@
       </x:c>
       <x:c r="G13" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I13" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:10">
       <x:c r="A14" s="0" t="n">
-        <x:v>1011</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C14" s="2">
-        <x:v>44327.7889103241</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>4</x:v>
@@ -1142,20 +1148,17 @@
       </x:c>
       <x:c r="G14" s="0" t="b">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="I14" s="0" t="s">
-        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10">
       <x:c r="A15" s="0" t="n">
-        <x:v>1012</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C15" s="2">
-        <x:v>44327.7896717014</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>4</x:v>
@@ -1172,13 +1175,13 @@
     </x:row>
     <x:row r="16" spans="1:10">
       <x:c r="A16" s="0" t="n">
-        <x:v>1013</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C16" s="2">
-        <x:v>44327.7898875116</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>4</x:v>
@@ -1195,13 +1198,13 @@
     </x:row>
     <x:row r="17" spans="1:10">
       <x:c r="A17" s="0" t="n">
-        <x:v>1014</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C17" s="2">
-        <x:v>44327.7900773148</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>4</x:v>
@@ -1218,13 +1221,13 @@
     </x:row>
     <x:row r="18" spans="1:10">
       <x:c r="A18" s="0" t="n">
-        <x:v>1015</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C18" s="2">
-        <x:v>44327.7902346644</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>4</x:v>
@@ -1241,13 +1244,13 @@
     </x:row>
     <x:row r="19" spans="1:10">
       <x:c r="A19" s="0" t="n">
-        <x:v>1016</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C19" s="2">
-        <x:v>44327.7905140393</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>4</x:v>
@@ -1264,13 +1267,13 @@
     </x:row>
     <x:row r="20" spans="1:10">
       <x:c r="A20" s="0" t="n">
-        <x:v>1017</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C20" s="2">
-        <x:v>44327.7906821875</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>4</x:v>
@@ -1287,13 +1290,13 @@
     </x:row>
     <x:row r="21" spans="1:10">
       <x:c r="A21" s="0" t="n">
-        <x:v>1018</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C21" s="2">
-        <x:v>44327.7908281944</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>4</x:v>
@@ -1310,13 +1313,13 @@
     </x:row>
     <x:row r="22" spans="1:10">
       <x:c r="A22" s="0" t="n">
-        <x:v>1019</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B22" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C22" s="2">
-        <x:v>44327.7909767708</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
         <x:v>4</x:v>
@@ -1333,13 +1336,13 @@
     </x:row>
     <x:row r="23" spans="1:10">
       <x:c r="A23" s="0" t="n">
-        <x:v>1020</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B23" s="1">
-        <x:v>44327</x:v>
+        <x:v>44320</x:v>
       </x:c>
       <x:c r="C23" s="2">
-        <x:v>44327.7911247338</x:v>
+        <x:v>44320.3703009259</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>4</x:v>
@@ -1351,6 +1354,305 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="G23" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:10">
+      <x:c r="A24" s="0" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B24" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C24" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G24" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:10">
+      <x:c r="A25" s="0" t="n">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B25" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C25" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G25" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:10">
+      <x:c r="A26" s="0" t="n">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B26" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C26" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G26" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:10">
+      <x:c r="A27" s="0" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B27" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C27" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G27" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:10">
+      <x:c r="A28" s="0" t="n">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B28" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C28" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G28" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:10">
+      <x:c r="A29" s="0" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B29" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C29" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G29" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:10">
+      <x:c r="A30" s="0" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B30" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C30" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G30" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:10">
+      <x:c r="A31" s="0" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B31" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C31" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G31" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:10">
+      <x:c r="A32" s="0" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B32" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C32" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G32" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:10">
+      <x:c r="A33" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B33" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C33" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G33" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:10">
+      <x:c r="A34" s="0" t="n">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B34" s="1">
+        <x:v>44320</x:v>
+      </x:c>
+      <x:c r="C34" s="2">
+        <x:v>44320.3703009259</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G34" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:10">
+      <x:c r="A35" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B35" s="1">
+        <x:v>44328</x:v>
+      </x:c>
+      <x:c r="C35" s="2">
+        <x:v>44328.375959213</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G35" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:10">
+      <x:c r="A36" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B36" s="1">
+        <x:v>44328</x:v>
+      </x:c>
+      <x:c r="C36" s="2">
+        <x:v>44328.3769489583</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="b">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G36" s="0" t="b">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1370,7 +1672,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F3"/>
+  <x:dimension ref="A1:F5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -1381,7 +1683,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
         <x:v>15</x:v>
@@ -1390,7 +1692,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
         <x:v>21</x:v>
@@ -1398,24 +1700,70 @@
     </x:row>
     <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="n">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>44319.7581985185</x:v>
+        <x:v>44320.3708740625</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C3" s="2">
+        <x:v>44320.9065409606</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C4" s="2">
+        <x:v>44320.9875444792</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C3" s="2">
-        <x:v>44319.7585063773</x:v>
+      <x:c r="C5" s="2">
+        <x:v>44327.90628625</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>